<commit_message>
Created placeholder for all new required authentication tests
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Repositories\rbk-api-modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C194E2E3-0E1D-4688-93E5-CC01EF71D547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64A2601-C6F7-4A0F-A379-C942FF1D65DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD3BEFF9-B2A9-4792-94FC-69A27E7F1E45}"/>
+    <workbookView xWindow="2400" yWindow="1950" windowWidth="25140" windowHeight="10575" xr2:uid="{CD3BEFF9-B2A9-4792-94FC-69A27E7F1E45}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="499">
   <si>
     <t>Tenants</t>
   </si>
@@ -1418,13 +1418,142 @@
   </si>
   <si>
     <t>IT-226</t>
+  </si>
+  <si>
+    <t>User cannot be created if username is not supplied</t>
+  </si>
+  <si>
+    <t>User cannot be created if email is not supplied</t>
+  </si>
+  <si>
+    <t>User cannot be created if email is invalid</t>
+  </si>
+  <si>
+    <t>User cannot be created if display name is not supplied</t>
+  </si>
+  <si>
+    <t>User cannot be created if custom metadata validations are not met</t>
+  </si>
+  <si>
+    <t>User cannot be created if password is not supplied</t>
+  </si>
+  <si>
+    <t>User cannot be created if passwords do not metch</t>
+  </si>
+  <si>
+    <t>User cannot be created if no role is supplied</t>
+  </si>
+  <si>
+    <t>User cannot be created if requesting user doesn't have the proper access rights</t>
+  </si>
+  <si>
+    <t>User can be created</t>
+  </si>
+  <si>
+    <t>IT-237</t>
+  </si>
+  <si>
+    <t>IT-236</t>
+  </si>
+  <si>
+    <t>IT-227</t>
+  </si>
+  <si>
+    <t>IT-228</t>
+  </si>
+  <si>
+    <t>IT-229</t>
+  </si>
+  <si>
+    <t>IT-232</t>
+  </si>
+  <si>
+    <t>IT-233</t>
+  </si>
+  <si>
+    <t>IT-234</t>
+  </si>
+  <si>
+    <t>IT-235</t>
+  </si>
+  <si>
+    <t>IT-250</t>
+  </si>
+  <si>
+    <t>IT-251</t>
+  </si>
+  <si>
+    <t>IT-252</t>
+  </si>
+  <si>
+    <t>IT-253</t>
+  </si>
+  <si>
+    <t>IT-254</t>
+  </si>
+  <si>
+    <t>IT-255</t>
+  </si>
+  <si>
+    <t>IT-256</t>
+  </si>
+  <si>
+    <t>IT-257</t>
+  </si>
+  <si>
+    <t>IT-258</t>
+  </si>
+  <si>
+    <t>IT-259</t>
+  </si>
+  <si>
+    <t>IT-260</t>
+  </si>
+  <si>
+    <t>IT-261</t>
+  </si>
+  <si>
+    <t>User cannot register if username is not provided</t>
+  </si>
+  <si>
+    <t>User cannot register if username is already taken</t>
+  </si>
+  <si>
+    <t>User cannot register if tenant does not exist</t>
+  </si>
+  <si>
+    <t>User cannot register if tenant is not provided</t>
+  </si>
+  <si>
+    <t>User cannot register if email is not provided</t>
+  </si>
+  <si>
+    <t>User cannot register if email is not valid</t>
+  </si>
+  <si>
+    <t>User cannot register if tenant is display name is not provided</t>
+  </si>
+  <si>
+    <t>User cannot register if metadata custom validators are not met</t>
+  </si>
+  <si>
+    <t>User cannot register if password is not provided</t>
+  </si>
+  <si>
+    <t>User cannot register if passwords don't match</t>
+  </si>
+  <si>
+    <t>User cannot register if passwords custom policies are not met</t>
+  </si>
+  <si>
+    <t>User can register</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1463,6 +1592,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2226,11 +2361,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55BE1F5-44A9-4975-A641-3A0C97931E70}">
-  <dimension ref="A1:K180"/>
+  <dimension ref="A1:K219"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A173" sqref="A173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6698,112 +6833,856 @@
       <c r="J171" s="32"/>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A172" s="29"/>
-      <c r="B172" s="30"/>
+      <c r="A172" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="B172" s="30" t="s">
+        <v>468</v>
+      </c>
       <c r="C172" s="30"/>
-      <c r="D172" s="30"/>
-      <c r="E172" s="30"/>
-      <c r="F172" s="30"/>
-      <c r="G172" s="30"/>
+      <c r="D172" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E172" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F172" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G172" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H172" s="31"/>
       <c r="I172" s="31"/>
       <c r="J172" s="32"/>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A173" s="29"/>
-      <c r="B173" s="30"/>
+      <c r="A173" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="B173" s="30" t="s">
+        <v>469</v>
+      </c>
       <c r="C173" s="30"/>
-      <c r="D173" s="30"/>
-      <c r="E173" s="30"/>
-      <c r="F173" s="30"/>
-      <c r="G173" s="30"/>
+      <c r="D173" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E173" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F173" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G173" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H173" s="31"/>
       <c r="I173" s="31"/>
       <c r="J173" s="32"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A174" s="29"/>
-      <c r="B174" s="30"/>
+      <c r="A174" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="B174" s="30" t="s">
+        <v>470</v>
+      </c>
       <c r="C174" s="30"/>
-      <c r="D174" s="30"/>
-      <c r="E174" s="30"/>
-      <c r="F174" s="30"/>
-      <c r="G174" s="30"/>
+      <c r="D174" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E174" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F174" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G174" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H174" s="31"/>
       <c r="I174" s="31"/>
       <c r="J174" s="32"/>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A175" s="29"/>
-      <c r="B175" s="30"/>
+      <c r="A175" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="B175" s="30" t="s">
+        <v>328</v>
+      </c>
       <c r="C175" s="30"/>
-      <c r="D175" s="30"/>
-      <c r="E175" s="30"/>
-      <c r="F175" s="30"/>
-      <c r="G175" s="30"/>
+      <c r="D175" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E175" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F175" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G175" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H175" s="31"/>
       <c r="I175" s="31"/>
       <c r="J175" s="32"/>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A176" s="29"/>
-      <c r="B176" s="30"/>
+      <c r="A176" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="B176" s="30" t="s">
+        <v>329</v>
+      </c>
       <c r="C176" s="30"/>
-      <c r="D176" s="30"/>
-      <c r="E176" s="30"/>
-      <c r="F176" s="30"/>
-      <c r="G176" s="30"/>
+      <c r="D176" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E176" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F176" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G176" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H176" s="31"/>
       <c r="I176" s="31"/>
       <c r="J176" s="32"/>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" s="29"/>
-      <c r="B177" s="30"/>
+      <c r="A177" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="B177" s="30" t="s">
+        <v>471</v>
+      </c>
       <c r="C177" s="30"/>
-      <c r="D177" s="30"/>
-      <c r="E177" s="30"/>
-      <c r="F177" s="30"/>
-      <c r="G177" s="30"/>
+      <c r="D177" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E177" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F177" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G177" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H177" s="31"/>
       <c r="I177" s="31"/>
       <c r="J177" s="32"/>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" s="29"/>
-      <c r="B178" s="30"/>
+      <c r="A178" s="29" t="s">
+        <v>461</v>
+      </c>
+      <c r="B178" s="30" t="s">
+        <v>472</v>
+      </c>
       <c r="C178" s="30"/>
-      <c r="D178" s="30"/>
-      <c r="E178" s="30"/>
-      <c r="F178" s="30"/>
-      <c r="G178" s="30"/>
+      <c r="D178" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E178" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F178" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G178" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H178" s="31"/>
       <c r="I178" s="31"/>
       <c r="J178" s="32"/>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" s="29"/>
-      <c r="B179" s="30"/>
+      <c r="A179" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="B179" s="30" t="s">
+        <v>473</v>
+      </c>
       <c r="C179" s="30"/>
-      <c r="D179" s="30"/>
-      <c r="E179" s="30"/>
-      <c r="F179" s="30"/>
-      <c r="G179" s="30"/>
+      <c r="D179" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E179" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F179" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G179" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H179" s="31"/>
       <c r="I179" s="31"/>
       <c r="J179" s="32"/>
     </row>
-    <row r="180" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="2"/>
-      <c r="B180" s="27"/>
-      <c r="C180" s="27"/>
-      <c r="D180" s="27"/>
-      <c r="E180" s="27"/>
-      <c r="F180" s="27"/>
-      <c r="G180" s="27"/>
-      <c r="H180" s="3"/>
-      <c r="I180" s="3"/>
-      <c r="J180" s="4"/>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="B180" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="C180" s="30"/>
+      <c r="D180" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E180" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F180" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G180" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H180" s="31"/>
+      <c r="I180" s="31"/>
+      <c r="J180" s="32"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="29" t="s">
+        <v>464</v>
+      </c>
+      <c r="B181" s="30" t="s">
+        <v>467</v>
+      </c>
+      <c r="C181" s="30"/>
+      <c r="D181" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E181" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F181" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G181" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H181" s="31"/>
+      <c r="I181" s="31"/>
+      <c r="J181" s="32"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="B182" s="30" t="s">
+        <v>466</v>
+      </c>
+      <c r="C182" s="30"/>
+      <c r="D182" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E182" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F182" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G182" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H182" s="31"/>
+      <c r="I182" s="31"/>
+      <c r="J182" s="32"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="B183" s="30" t="s">
+        <v>475</v>
+      </c>
+      <c r="C183" s="30"/>
+      <c r="D183" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E183" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F183" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G183" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H183" s="31"/>
+      <c r="I183" s="31"/>
+      <c r="J183" s="32"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" s="29" t="s">
+        <v>488</v>
+      </c>
+      <c r="B184" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="C184" s="30"/>
+      <c r="D184" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E184" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F184" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G184" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H184" s="31"/>
+      <c r="I184" s="31"/>
+      <c r="J184" s="32"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="29" t="s">
+        <v>489</v>
+      </c>
+      <c r="B185" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="C185" s="30"/>
+      <c r="D185" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E185" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F185" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G185" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H185" s="31"/>
+      <c r="I185" s="31"/>
+      <c r="J185" s="32"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="B186" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="C186" s="30"/>
+      <c r="D186" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E186" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F186" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G186" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H186" s="31"/>
+      <c r="I186" s="31"/>
+      <c r="J186" s="32"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="29" t="s">
+        <v>491</v>
+      </c>
+      <c r="B187" s="30" t="s">
+        <v>479</v>
+      </c>
+      <c r="C187" s="30"/>
+      <c r="D187" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E187" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F187" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G187" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H187" s="31"/>
+      <c r="I187" s="31"/>
+      <c r="J187" s="32"/>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="29" t="s">
+        <v>492</v>
+      </c>
+      <c r="B188" s="30" t="s">
+        <v>480</v>
+      </c>
+      <c r="C188" s="30"/>
+      <c r="D188" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E188" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F188" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G188" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H188" s="31"/>
+      <c r="I188" s="31"/>
+      <c r="J188" s="32"/>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="B189" s="30" t="s">
+        <v>481</v>
+      </c>
+      <c r="C189" s="30"/>
+      <c r="D189" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E189" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F189" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G189" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H189" s="31"/>
+      <c r="I189" s="31"/>
+      <c r="J189" s="32"/>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="29" t="s">
+        <v>494</v>
+      </c>
+      <c r="B190" s="30" t="s">
+        <v>482</v>
+      </c>
+      <c r="C190" s="30"/>
+      <c r="D190" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E190" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F190" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G190" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H190" s="31"/>
+      <c r="I190" s="31"/>
+      <c r="J190" s="32"/>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="B191" s="30" t="s">
+        <v>483</v>
+      </c>
+      <c r="C191" s="30"/>
+      <c r="D191" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E191" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F191" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G191" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H191" s="31"/>
+      <c r="I191" s="31"/>
+      <c r="J191" s="32"/>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" s="29" t="s">
+        <v>496</v>
+      </c>
+      <c r="B192" s="30" t="s">
+        <v>484</v>
+      </c>
+      <c r="C192" s="30"/>
+      <c r="D192" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E192" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F192" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G192" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H192" s="31"/>
+      <c r="I192" s="31"/>
+      <c r="J192" s="32"/>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="29" t="s">
+        <v>497</v>
+      </c>
+      <c r="B193" s="30" t="s">
+        <v>485</v>
+      </c>
+      <c r="C193" s="30"/>
+      <c r="D193" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E193" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F193" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G193" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H193" s="31"/>
+      <c r="I193" s="31"/>
+      <c r="J193" s="32"/>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" s="29" t="s">
+        <v>498</v>
+      </c>
+      <c r="B194" s="30" t="s">
+        <v>486</v>
+      </c>
+      <c r="C194" s="30"/>
+      <c r="D194" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E194" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F194" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G194" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H194" s="31"/>
+      <c r="I194" s="31"/>
+      <c r="J194" s="32"/>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" s="29"/>
+      <c r="B195" s="30"/>
+      <c r="C195" s="30"/>
+      <c r="D195" s="30"/>
+      <c r="E195" s="30"/>
+      <c r="F195" s="30"/>
+      <c r="G195" s="30"/>
+      <c r="H195" s="31"/>
+      <c r="I195" s="31"/>
+      <c r="J195" s="32"/>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" s="29"/>
+      <c r="B196" s="30"/>
+      <c r="C196" s="30"/>
+      <c r="D196" s="30"/>
+      <c r="E196" s="30"/>
+      <c r="F196" s="30"/>
+      <c r="G196" s="30"/>
+      <c r="H196" s="31"/>
+      <c r="I196" s="31"/>
+      <c r="J196" s="32"/>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" s="29"/>
+      <c r="B197" s="30"/>
+      <c r="C197" s="30"/>
+      <c r="D197" s="30"/>
+      <c r="E197" s="30"/>
+      <c r="F197" s="30"/>
+      <c r="G197" s="30"/>
+      <c r="H197" s="31"/>
+      <c r="I197" s="31"/>
+      <c r="J197" s="32"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="29"/>
+      <c r="B198" s="30"/>
+      <c r="C198" s="30"/>
+      <c r="D198" s="30"/>
+      <c r="E198" s="30"/>
+      <c r="F198" s="30"/>
+      <c r="G198" s="30"/>
+      <c r="H198" s="31"/>
+      <c r="I198" s="31"/>
+      <c r="J198" s="32"/>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" s="29"/>
+      <c r="B199" s="30"/>
+      <c r="C199" s="30"/>
+      <c r="D199" s="30"/>
+      <c r="E199" s="30"/>
+      <c r="F199" s="30"/>
+      <c r="G199" s="30"/>
+      <c r="H199" s="31"/>
+      <c r="I199" s="31"/>
+      <c r="J199" s="32"/>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" s="29"/>
+      <c r="B200" s="30"/>
+      <c r="C200" s="30"/>
+      <c r="D200" s="30"/>
+      <c r="E200" s="30"/>
+      <c r="F200" s="30"/>
+      <c r="G200" s="30"/>
+      <c r="H200" s="31"/>
+      <c r="I200" s="31"/>
+      <c r="J200" s="32"/>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" s="29"/>
+      <c r="B201" s="30"/>
+      <c r="C201" s="30"/>
+      <c r="D201" s="30"/>
+      <c r="E201" s="30"/>
+      <c r="F201" s="30"/>
+      <c r="G201" s="30"/>
+      <c r="H201" s="31"/>
+      <c r="I201" s="31"/>
+      <c r="J201" s="32"/>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="29"/>
+      <c r="B202" s="30"/>
+      <c r="C202" s="30"/>
+      <c r="D202" s="30"/>
+      <c r="E202" s="30"/>
+      <c r="F202" s="30"/>
+      <c r="G202" s="30"/>
+      <c r="H202" s="31"/>
+      <c r="I202" s="31"/>
+      <c r="J202" s="32"/>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="29"/>
+      <c r="B203" s="30"/>
+      <c r="C203" s="30"/>
+      <c r="D203" s="30"/>
+      <c r="E203" s="30"/>
+      <c r="F203" s="30"/>
+      <c r="G203" s="30"/>
+      <c r="H203" s="31"/>
+      <c r="I203" s="31"/>
+      <c r="J203" s="32"/>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="29"/>
+      <c r="B204" s="30"/>
+      <c r="C204" s="30"/>
+      <c r="D204" s="30"/>
+      <c r="E204" s="30"/>
+      <c r="F204" s="30"/>
+      <c r="G204" s="30"/>
+      <c r="H204" s="31"/>
+      <c r="I204" s="31"/>
+      <c r="J204" s="32"/>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" s="29"/>
+      <c r="B205" s="30"/>
+      <c r="C205" s="30"/>
+      <c r="D205" s="30"/>
+      <c r="E205" s="30"/>
+      <c r="F205" s="30"/>
+      <c r="G205" s="30"/>
+      <c r="H205" s="31"/>
+      <c r="I205" s="31"/>
+      <c r="J205" s="32"/>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" s="29"/>
+      <c r="B206" s="30"/>
+      <c r="C206" s="30"/>
+      <c r="D206" s="30"/>
+      <c r="E206" s="30"/>
+      <c r="F206" s="30"/>
+      <c r="G206" s="30"/>
+      <c r="H206" s="31"/>
+      <c r="I206" s="31"/>
+      <c r="J206" s="32"/>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="29"/>
+      <c r="B207" s="30"/>
+      <c r="C207" s="30"/>
+      <c r="D207" s="30"/>
+      <c r="E207" s="30"/>
+      <c r="F207" s="30"/>
+      <c r="G207" s="30"/>
+      <c r="H207" s="31"/>
+      <c r="I207" s="31"/>
+      <c r="J207" s="32"/>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="29"/>
+      <c r="B208" s="30"/>
+      <c r="C208" s="30"/>
+      <c r="D208" s="30"/>
+      <c r="E208" s="30"/>
+      <c r="F208" s="30"/>
+      <c r="G208" s="30"/>
+      <c r="H208" s="31"/>
+      <c r="I208" s="31"/>
+      <c r="J208" s="32"/>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209" s="29"/>
+      <c r="B209" s="30"/>
+      <c r="C209" s="30"/>
+      <c r="D209" s="30"/>
+      <c r="E209" s="30"/>
+      <c r="F209" s="30"/>
+      <c r="G209" s="30"/>
+      <c r="H209" s="31"/>
+      <c r="I209" s="31"/>
+      <c r="J209" s="32"/>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210" s="29"/>
+      <c r="B210" s="30"/>
+      <c r="C210" s="30"/>
+      <c r="D210" s="30"/>
+      <c r="E210" s="30"/>
+      <c r="F210" s="30"/>
+      <c r="G210" s="30"/>
+      <c r="H210" s="31"/>
+      <c r="I210" s="31"/>
+      <c r="J210" s="32"/>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211" s="29"/>
+      <c r="B211" s="30"/>
+      <c r="C211" s="30"/>
+      <c r="D211" s="30"/>
+      <c r="E211" s="30"/>
+      <c r="F211" s="30"/>
+      <c r="G211" s="30"/>
+      <c r="H211" s="31"/>
+      <c r="I211" s="31"/>
+      <c r="J211" s="32"/>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212" s="29"/>
+      <c r="B212" s="30"/>
+      <c r="C212" s="30"/>
+      <c r="D212" s="30"/>
+      <c r="E212" s="30"/>
+      <c r="F212" s="30"/>
+      <c r="G212" s="30"/>
+      <c r="H212" s="31"/>
+      <c r="I212" s="31"/>
+      <c r="J212" s="32"/>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213" s="29"/>
+      <c r="B213" s="30"/>
+      <c r="C213" s="30"/>
+      <c r="D213" s="30"/>
+      <c r="E213" s="30"/>
+      <c r="F213" s="30"/>
+      <c r="G213" s="30"/>
+      <c r="H213" s="31"/>
+      <c r="I213" s="31"/>
+      <c r="J213" s="32"/>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214" s="29"/>
+      <c r="B214" s="30"/>
+      <c r="C214" s="30"/>
+      <c r="D214" s="30"/>
+      <c r="E214" s="30"/>
+      <c r="F214" s="30"/>
+      <c r="G214" s="30"/>
+      <c r="H214" s="31"/>
+      <c r="I214" s="31"/>
+      <c r="J214" s="32"/>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" s="29"/>
+      <c r="B215" s="30"/>
+      <c r="C215" s="30"/>
+      <c r="D215" s="30"/>
+      <c r="E215" s="30"/>
+      <c r="F215" s="30"/>
+      <c r="G215" s="30"/>
+      <c r="H215" s="31"/>
+      <c r="I215" s="31"/>
+      <c r="J215" s="32"/>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" s="29"/>
+      <c r="B216" s="30"/>
+      <c r="C216" s="30"/>
+      <c r="D216" s="30"/>
+      <c r="E216" s="30"/>
+      <c r="F216" s="30"/>
+      <c r="G216" s="30"/>
+      <c r="H216" s="31"/>
+      <c r="I216" s="31"/>
+      <c r="J216" s="32"/>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" s="29"/>
+      <c r="B217" s="30"/>
+      <c r="C217" s="30"/>
+      <c r="D217" s="30"/>
+      <c r="E217" s="30"/>
+      <c r="F217" s="30"/>
+      <c r="G217" s="30"/>
+      <c r="H217" s="31"/>
+      <c r="I217" s="31"/>
+      <c r="J217" s="32"/>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218" s="29"/>
+      <c r="B218" s="30"/>
+      <c r="C218" s="30"/>
+      <c r="D218" s="30"/>
+      <c r="E218" s="30"/>
+      <c r="F218" s="30"/>
+      <c r="G218" s="30"/>
+      <c r="H218" s="31"/>
+      <c r="I218" s="31"/>
+      <c r="J218" s="32"/>
+    </row>
+    <row r="219" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="2"/>
+      <c r="B219" s="27"/>
+      <c r="C219" s="27"/>
+      <c r="D219" s="27"/>
+      <c r="E219" s="27"/>
+      <c r="F219" s="27"/>
+      <c r="G219" s="27"/>
+      <c r="H219" s="3"/>
+      <c r="I219" s="3"/>
+      <c r="J219" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J163" xr:uid="{F55BE1F5-44A9-4975-A641-3A0C97931E70}"/>
@@ -6814,6 +7693,7 @@
     <sortCondition ref="B2:B148"/>
     <sortCondition ref="F2:F148"/>
   </sortState>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Some Windows Authentication tests and namespace refactory on test projects
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Repositories\rbk-api-modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64A2601-C6F7-4A0F-A379-C942FF1D65DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B758C120-E369-4BEF-A48E-F8E2A7F67906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1950" windowWidth="25140" windowHeight="10575" xr2:uid="{CD3BEFF9-B2A9-4792-94FC-69A27E7F1E45}"/>
+    <workbookView xWindow="2400" yWindow="1950" windowWidth="26055" windowHeight="10575" xr2:uid="{CD3BEFF9-B2A9-4792-94FC-69A27E7F1E45}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="525">
   <si>
     <t>Tenants</t>
   </si>
@@ -1441,9 +1441,6 @@
     <t>User cannot be created if passwords do not metch</t>
   </si>
   <si>
-    <t>User cannot be created if no role is supplied</t>
-  </si>
-  <si>
     <t>User cannot be created if requesting user doesn't have the proper access rights</t>
   </si>
   <si>
@@ -1547,6 +1544,87 @@
   </si>
   <si>
     <t>User can register</t>
+  </si>
+  <si>
+    <t>User cannot be created if no role is supplied (null list)</t>
+  </si>
+  <si>
+    <t>User cannot be created if no role is supplied (empty list)</t>
+  </si>
+  <si>
+    <t>IT-239</t>
+  </si>
+  <si>
+    <t>User cannot be created if role list has an invalid role</t>
+  </si>
+  <si>
+    <t>IT-240</t>
+  </si>
+  <si>
+    <t>With Windows Authentication  redefine password endpoint should not be available</t>
+  </si>
+  <si>
+    <t>With Windows Authentication  reset password  endpoint should not be available</t>
+  </si>
+  <si>
+    <t>With Windows Authentication resend confirmation endpoint should not be available</t>
+  </si>
+  <si>
+    <t>With Windows Authentication confirm e-mail  endpoint should not be available</t>
+  </si>
+  <si>
+    <t>With Windows Authentication change password endpoint should not be available</t>
+  </si>
+  <si>
+    <t>With Windows Authentication register endpoint should not be available</t>
+  </si>
+  <si>
+    <t>Without Windows Authentication switch domain endpoint should not be available</t>
+  </si>
+  <si>
+    <t>Without Windows Authentication create user endpoint should not be available</t>
+  </si>
+  <si>
+    <t>IT-270</t>
+  </si>
+  <si>
+    <t>IT-271</t>
+  </si>
+  <si>
+    <t>IT-272</t>
+  </si>
+  <si>
+    <t>IT-273</t>
+  </si>
+  <si>
+    <t>IT-274</t>
+  </si>
+  <si>
+    <t>IT-275</t>
+  </si>
+  <si>
+    <t>IT-290</t>
+  </si>
+  <si>
+    <t>IT-291</t>
+  </si>
+  <si>
+    <t>With Windows Authentication user cannot login if it passes a custom login validator but doesn't exist in database</t>
+  </si>
+  <si>
+    <t>IT-262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With Windows Authentication user cannot login if it doesn't pass a a custom login validator </t>
+  </si>
+  <si>
+    <t>IT-263</t>
+  </si>
+  <si>
+    <t>With Windows Authentication user can login if all conditions are met</t>
+  </si>
+  <si>
+    <t>IT-264</t>
   </si>
 </sst>
 </file>
@@ -2361,16 +2439,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55BE1F5-44A9-4975-A641-3A0C97931E70}">
-  <dimension ref="A1:K219"/>
+  <dimension ref="A1:K221"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A173" sqref="A173"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A204" sqref="A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="93.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="28" customWidth="1"/>
     <col min="3" max="3" width="9" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="28" bestFit="1" customWidth="1"/>
@@ -6837,7 +6915,7 @@
         <v>456</v>
       </c>
       <c r="B172" s="30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C172" s="30"/>
       <c r="D172" s="30" t="s">
@@ -6861,7 +6939,7 @@
         <v>456</v>
       </c>
       <c r="B173" s="30" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C173" s="30"/>
       <c r="D173" s="30" t="s">
@@ -6885,7 +6963,7 @@
         <v>457</v>
       </c>
       <c r="B174" s="30" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C174" s="30"/>
       <c r="D174" s="30" t="s">
@@ -6957,7 +7035,7 @@
         <v>460</v>
       </c>
       <c r="B177" s="30" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C177" s="30"/>
       <c r="D177" s="30" t="s">
@@ -6981,7 +7059,7 @@
         <v>461</v>
       </c>
       <c r="B178" s="30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C178" s="30"/>
       <c r="D178" s="30" t="s">
@@ -7005,7 +7083,7 @@
         <v>462</v>
       </c>
       <c r="B179" s="30" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C179" s="30"/>
       <c r="D179" s="30" t="s">
@@ -7026,10 +7104,10 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="29" t="s">
-        <v>463</v>
+        <v>498</v>
       </c>
       <c r="B180" s="30" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C180" s="30"/>
       <c r="D180" s="30" t="s">
@@ -7050,10 +7128,10 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="29" t="s">
-        <v>464</v>
+        <v>499</v>
       </c>
       <c r="B181" s="30" t="s">
-        <v>467</v>
+        <v>500</v>
       </c>
       <c r="C181" s="30"/>
       <c r="D181" s="30" t="s">
@@ -7074,10 +7152,10 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="29" t="s">
-        <v>465</v>
+        <v>501</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>466</v>
+        <v>502</v>
       </c>
       <c r="C182" s="30"/>
       <c r="D182" s="30" t="s">
@@ -7090,7 +7168,7 @@
         <v>46</v>
       </c>
       <c r="G182" s="30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H182" s="31"/>
       <c r="I182" s="31"/>
@@ -7098,10 +7176,10 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="29" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="B183" s="30" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="C183" s="30"/>
       <c r="D183" s="30" t="s">
@@ -7122,10 +7200,10 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="29" t="s">
-        <v>488</v>
+        <v>464</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="C184" s="30"/>
       <c r="D184" s="30" t="s">
@@ -7138,7 +7216,7 @@
         <v>46</v>
       </c>
       <c r="G184" s="30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H184" s="31"/>
       <c r="I184" s="31"/>
@@ -7146,10 +7224,10 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="29" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C185" s="30"/>
       <c r="D185" s="30" t="s">
@@ -7170,10 +7248,10 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="29" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B186" s="30" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C186" s="30"/>
       <c r="D186" s="30" t="s">
@@ -7194,10 +7272,10 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="29" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B187" s="30" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C187" s="30"/>
       <c r="D187" s="30" t="s">
@@ -7218,10 +7296,10 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="29" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B188" s="30" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C188" s="30"/>
       <c r="D188" s="30" t="s">
@@ -7242,10 +7320,10 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="29" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B189" s="30" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C189" s="30"/>
       <c r="D189" s="30" t="s">
@@ -7266,10 +7344,10 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="29" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C190" s="30"/>
       <c r="D190" s="30" t="s">
@@ -7290,10 +7368,10 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B191" s="30" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C191" s="30"/>
       <c r="D191" s="30" t="s">
@@ -7314,10 +7392,10 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="29" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B192" s="30" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C192" s="30"/>
       <c r="D192" s="30" t="s">
@@ -7338,10 +7416,10 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="29" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B193" s="30" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C193" s="30"/>
       <c r="D193" s="30" t="s">
@@ -7362,10 +7440,10 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B194" s="30" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C194" s="30"/>
       <c r="D194" s="30" t="s">
@@ -7378,140 +7456,278 @@
         <v>46</v>
       </c>
       <c r="G194" s="30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H194" s="31"/>
       <c r="I194" s="31"/>
       <c r="J194" s="32"/>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A195" s="29"/>
-      <c r="B195" s="30"/>
+      <c r="A195" s="29" t="s">
+        <v>496</v>
+      </c>
+      <c r="B195" s="30" t="s">
+        <v>484</v>
+      </c>
       <c r="C195" s="30"/>
-      <c r="D195" s="30"/>
-      <c r="E195" s="30"/>
-      <c r="F195" s="30"/>
-      <c r="G195" s="30"/>
+      <c r="D195" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E195" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F195" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G195" s="30" t="s">
+        <v>5</v>
+      </c>
       <c r="H195" s="31"/>
       <c r="I195" s="31"/>
       <c r="J195" s="32"/>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A196" s="29"/>
-      <c r="B196" s="30"/>
+      <c r="A196" s="29" t="s">
+        <v>497</v>
+      </c>
+      <c r="B196" s="30" t="s">
+        <v>485</v>
+      </c>
       <c r="C196" s="30"/>
-      <c r="D196" s="30"/>
-      <c r="E196" s="30"/>
-      <c r="F196" s="30"/>
-      <c r="G196" s="30"/>
+      <c r="D196" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E196" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F196" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="G196" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H196" s="31"/>
       <c r="I196" s="31"/>
       <c r="J196" s="32"/>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A197" s="29"/>
-      <c r="B197" s="30"/>
-      <c r="C197" s="30"/>
-      <c r="D197" s="30"/>
-      <c r="E197" s="30"/>
-      <c r="F197" s="30"/>
-      <c r="G197" s="30"/>
-      <c r="H197" s="31"/>
-      <c r="I197" s="31"/>
-      <c r="J197" s="32"/>
+      <c r="A197" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="B197" s="34" t="s">
+        <v>524</v>
+      </c>
+      <c r="C197" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="D197" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="E197" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="F197" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G197" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H197" s="35"/>
+      <c r="I197" s="35"/>
+      <c r="J197" s="36"/>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A198" s="29"/>
-      <c r="B198" s="30"/>
-      <c r="C198" s="30"/>
-      <c r="D198" s="30"/>
-      <c r="E198" s="30"/>
-      <c r="F198" s="30"/>
-      <c r="G198" s="30"/>
-      <c r="H198" s="31"/>
-      <c r="I198" s="31"/>
-      <c r="J198" s="32"/>
+      <c r="A198" s="33" t="s">
+        <v>521</v>
+      </c>
+      <c r="B198" s="34" t="s">
+        <v>522</v>
+      </c>
+      <c r="C198" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="D198" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="E198" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="F198" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G198" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H198" s="35"/>
+      <c r="I198" s="35"/>
+      <c r="J198" s="36"/>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A199" s="29"/>
-      <c r="B199" s="30"/>
-      <c r="C199" s="30"/>
-      <c r="D199" s="30"/>
-      <c r="E199" s="30"/>
-      <c r="F199" s="30"/>
-      <c r="G199" s="30"/>
-      <c r="H199" s="31"/>
-      <c r="I199" s="31"/>
-      <c r="J199" s="32"/>
+      <c r="A199" s="33" t="s">
+        <v>519</v>
+      </c>
+      <c r="B199" s="34" t="s">
+        <v>520</v>
+      </c>
+      <c r="C199" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="D199" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="E199" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="F199" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G199" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H199" s="35"/>
+      <c r="I199" s="35"/>
+      <c r="J199" s="36"/>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A200" s="29"/>
-      <c r="B200" s="30"/>
+      <c r="A200" s="29" t="s">
+        <v>503</v>
+      </c>
+      <c r="B200" s="30" t="s">
+        <v>511</v>
+      </c>
       <c r="C200" s="30"/>
-      <c r="D200" s="30"/>
-      <c r="E200" s="30"/>
-      <c r="F200" s="30"/>
-      <c r="G200" s="30"/>
+      <c r="D200" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E200" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F200" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G200" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H200" s="31"/>
       <c r="I200" s="31"/>
       <c r="J200" s="32"/>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A201" s="29"/>
-      <c r="B201" s="30"/>
+      <c r="A201" s="29" t="s">
+        <v>504</v>
+      </c>
+      <c r="B201" s="30" t="s">
+        <v>512</v>
+      </c>
       <c r="C201" s="30"/>
-      <c r="D201" s="30"/>
-      <c r="E201" s="30"/>
-      <c r="F201" s="30"/>
-      <c r="G201" s="30"/>
+      <c r="D201" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E201" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F201" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G201" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H201" s="31"/>
       <c r="I201" s="31"/>
       <c r="J201" s="32"/>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A202" s="29"/>
-      <c r="B202" s="30"/>
+      <c r="A202" s="29" t="s">
+        <v>505</v>
+      </c>
+      <c r="B202" s="30" t="s">
+        <v>513</v>
+      </c>
       <c r="C202" s="30"/>
-      <c r="D202" s="30"/>
-      <c r="E202" s="30"/>
-      <c r="F202" s="30"/>
-      <c r="G202" s="30"/>
+      <c r="D202" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E202" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F202" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G202" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H202" s="31"/>
       <c r="I202" s="31"/>
       <c r="J202" s="32"/>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A203" s="29"/>
-      <c r="B203" s="30"/>
+      <c r="A203" s="29" t="s">
+        <v>506</v>
+      </c>
+      <c r="B203" s="30" t="s">
+        <v>514</v>
+      </c>
       <c r="C203" s="30"/>
-      <c r="D203" s="30"/>
-      <c r="E203" s="30"/>
-      <c r="F203" s="30"/>
-      <c r="G203" s="30"/>
+      <c r="D203" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E203" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F203" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G203" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H203" s="31"/>
       <c r="I203" s="31"/>
       <c r="J203" s="32"/>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A204" s="29"/>
-      <c r="B204" s="30"/>
+      <c r="A204" s="29" t="s">
+        <v>507</v>
+      </c>
+      <c r="B204" s="30" t="s">
+        <v>515</v>
+      </c>
       <c r="C204" s="30"/>
-      <c r="D204" s="30"/>
-      <c r="E204" s="30"/>
-      <c r="F204" s="30"/>
-      <c r="G204" s="30"/>
+      <c r="D204" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E204" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F204" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G204" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H204" s="31"/>
       <c r="I204" s="31"/>
       <c r="J204" s="32"/>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A205" s="29"/>
-      <c r="B205" s="30"/>
+      <c r="A205" s="29" t="s">
+        <v>508</v>
+      </c>
+      <c r="B205" s="30" t="s">
+        <v>516</v>
+      </c>
       <c r="C205" s="30"/>
-      <c r="D205" s="30"/>
-      <c r="E205" s="30"/>
-      <c r="F205" s="30"/>
-      <c r="G205" s="30"/>
+      <c r="D205" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E205" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F205" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G205" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H205" s="31"/>
       <c r="I205" s="31"/>
       <c r="J205" s="32"/>
@@ -7529,25 +7745,49 @@
       <c r="J206" s="32"/>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A207" s="29"/>
-      <c r="B207" s="30"/>
+      <c r="A207" s="29" t="s">
+        <v>509</v>
+      </c>
+      <c r="B207" s="30" t="s">
+        <v>517</v>
+      </c>
       <c r="C207" s="30"/>
-      <c r="D207" s="30"/>
-      <c r="E207" s="30"/>
-      <c r="F207" s="30"/>
-      <c r="G207" s="30"/>
+      <c r="D207" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E207" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F207" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G207" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H207" s="31"/>
       <c r="I207" s="31"/>
       <c r="J207" s="32"/>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A208" s="29"/>
-      <c r="B208" s="30"/>
+      <c r="A208" s="29" t="s">
+        <v>510</v>
+      </c>
+      <c r="B208" s="30" t="s">
+        <v>518</v>
+      </c>
       <c r="C208" s="30"/>
-      <c r="D208" s="30"/>
-      <c r="E208" s="30"/>
-      <c r="F208" s="30"/>
-      <c r="G208" s="30"/>
+      <c r="D208" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E208" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F208" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G208" s="30" t="s">
+        <v>4</v>
+      </c>
       <c r="H208" s="31"/>
       <c r="I208" s="31"/>
       <c r="J208" s="32"/>
@@ -7672,17 +7912,41 @@
       <c r="I218" s="31"/>
       <c r="J218" s="32"/>
     </row>
-    <row r="219" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="2"/>
-      <c r="B219" s="27"/>
-      <c r="C219" s="27"/>
-      <c r="D219" s="27"/>
-      <c r="E219" s="27"/>
-      <c r="F219" s="27"/>
-      <c r="G219" s="27"/>
-      <c r="H219" s="3"/>
-      <c r="I219" s="3"/>
-      <c r="J219" s="4"/>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219" s="29"/>
+      <c r="B219" s="30"/>
+      <c r="C219" s="30"/>
+      <c r="D219" s="30"/>
+      <c r="E219" s="30"/>
+      <c r="F219" s="30"/>
+      <c r="G219" s="30"/>
+      <c r="H219" s="31"/>
+      <c r="I219" s="31"/>
+      <c r="J219" s="32"/>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220" s="29"/>
+      <c r="B220" s="30"/>
+      <c r="C220" s="30"/>
+      <c r="D220" s="30"/>
+      <c r="E220" s="30"/>
+      <c r="F220" s="30"/>
+      <c r="G220" s="30"/>
+      <c r="H220" s="31"/>
+      <c r="I220" s="31"/>
+      <c r="J220" s="32"/>
+    </row>
+    <row r="221" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="2"/>
+      <c r="B221" s="27"/>
+      <c r="C221" s="27"/>
+      <c r="D221" s="27"/>
+      <c r="E221" s="27"/>
+      <c r="F221" s="27"/>
+      <c r="G221" s="27"/>
+      <c r="H221" s="3"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J163" xr:uid="{F55BE1F5-44A9-4975-A641-3A0C97931E70}"/>
@@ -7704,7 +7968,7 @@
   <dimension ref="A1:K172"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -10094,7 +10358,7 @@
   <dimension ref="A1:J171"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>